<commit_message>
udemy course material added
</commit_message>
<xml_diff>
--- a/angular-notes.xlsx
+++ b/angular-notes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YFukagawa/Documents/GitHub/angular-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BCB0F46-E6F0-4543-936A-AECC437DD429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC9A7F7-DA4B-FF45-98AE-3885C24412A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{B4CAA976-722B-0C4D-B978-4546B8B744B7}"/>
+    <workbookView xWindow="1240" yWindow="4820" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{B4CAA976-722B-0C4D-B978-4546B8B744B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="compiling" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,39 +37,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>just in time compilation</t>
   </si>
   <si>
-    <t>ahead of time compilation</t>
-  </si>
-  <si>
     <t>source code &gt;</t>
+  </si>
+  <si>
+    <t>Browser runs app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server </t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>JUST IN TIME COMPILATION</t>
+  </si>
+  <si>
+    <t>compiles when needed</t>
+  </si>
+  <si>
+    <t>compile code on the server</t>
+  </si>
+  <si>
+    <t>ahead of time compilation (AOT)</t>
+  </si>
+  <si>
+    <t>AHEAD OF TIME COMPILATION</t>
   </si>
   <si>
     <t>Templates &gt;
 Services
-Modules</t>
-  </si>
-  <si>
-    <t>Browser runs app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Server </t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>JUST IN TIME COMPILATION</t>
+Modules
+(ANGULAR COMPILER)</t>
+  </si>
+  <si>
+    <t>(typescript)</t>
+  </si>
+  <si>
+    <t>large file size</t>
+  </si>
+  <si>
+    <t>loads slower since compiler needs to run browser</t>
+  </si>
+  <si>
+    <t>small file size</t>
+  </si>
+  <si>
+    <t>load faster since the app is compiled on delivery to the browser</t>
+  </si>
+  <si>
+    <t>catch errors in browser</t>
+  </si>
+  <si>
+    <t>catch errors on the server</t>
+  </si>
+  <si>
+    <t>Angular is agnostic</t>
+  </si>
+  <si>
+    <t>build the platform, then can run on any operation system</t>
+  </si>
+  <si>
+    <t>ng serv</t>
+  </si>
+  <si>
+    <t>Development server, use the terminal command:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,16 +120,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -179,6 +243,46 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -190,27 +294,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,65 +667,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FAF974-15FC-8849-B9A2-81BC729D35E5}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="62" style="9" customWidth="1"/>
+    <col min="2" max="2" width="62" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="16" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05593B93-8071-3542-AF6D-46D13D475F50}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="65" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F4" s="3"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="5"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="6"/>
+    <row r="1" spans="1:2" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G3:G5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>